<commit_message>
Se agrego la implementacion de ColaEstatica y su clase Test.
</commit_message>
<xml_diff>
--- a/practica2/trunk/TDAs/doc/metricas/metricas_cola.xlsx
+++ b/practica2/trunk/TDAs/doc/metricas/metricas_cola.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="329"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Metricas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -92,20 +92,33 @@
   </si>
   <si>
     <t>TIEMPO EFECTIVO DESARROLLO</t>
+  </si>
+  <si>
+    <t>Crear interfaz Cola</t>
+  </si>
+  <si>
+    <t>Implementar Cola Estatica</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -145,6 +158,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -647,136 +668,142 @@
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="11" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="11" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="3" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="3" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="5" borderId="11" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="11" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="21" fontId="4" fillId="5" borderId="17" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="4" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="21" fontId="5" fillId="5" borderId="17" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="4" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="21" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="21" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="4" fillId="5" borderId="22" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="3" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="3" fillId="2" borderId="25" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="5" borderId="21" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="21" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="5" fillId="5" borderId="22" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="4" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="4" fillId="2" borderId="25" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="21" fontId="4" fillId="5" borderId="27" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="21" fontId="5" fillId="5" borderId="27" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="15" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="15" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="29" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="30" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="31" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="30" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="31" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="25" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="25" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="5" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -870,17 +897,8 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -899,9 +917,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -911,7 +927,6 @@
           <c:order val="0"/>
           <c:dPt>
             <c:idx val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
@@ -956,7 +971,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
@@ -1055,16 +1069,10 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-AR"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
             <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1087,23 +1095,17 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.05</c:v>
+                  <c:v>0.3846153846153843</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95</c:v>
+                  <c:v>0.61538461538461575</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
           <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="0"/>
         </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
@@ -1111,15 +1113,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.51180555555555551" footer="0.51180555555555551"/>
+    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.51180555555555562" footer="0.51180555555555562"/>
     <c:pageSetup firstPageNumber="0"/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1190,7 +1190,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
@@ -1198,7 +1198,7 @@
         <a:effectLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="77"/>
               </a:solidFill>
@@ -1208,7 +1208,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1257,7 +1257,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
@@ -1265,7 +1265,7 @@
         <a:effectLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="77"/>
               </a:solidFill>
@@ -1275,7 +1275,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1598,11 +1598,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -1612,7 +1612,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1640,11 +1640,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -1654,7 +1654,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1673,15 +1673,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:IU37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="34.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="34.28515625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="38.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" style="1" customWidth="1"/>
@@ -1696,7 +1696,7 @@
     <col min="11" max="255" width="34.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -1715,19 +1715,25 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15">
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="55">
+        <v>3.472222222222222E-3</v>
+      </c>
       <c r="C2" s="11">
         <f>E2-D2</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E2" s="12">
+        <v>0.4826388888888889</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -1739,8 +1745,8 @@
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
     </row>
-    <row r="4" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="13.5" thickBot="1"/>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1">
       <c r="A5" s="47" t="s">
         <v>6</v>
       </c>
@@ -1772,43 +1778,75 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+    <row r="6" spans="1:11" ht="15">
+      <c r="A6" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="16">
+        <v>7</v>
+      </c>
+      <c r="C6" s="16">
+        <v>7</v>
+      </c>
+      <c r="D6" s="17">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0.48958333333333331</v>
+      </c>
       <c r="G6" s="17">
         <f>F6-E6</f>
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="H6" s="16">
         <v>0</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17"/>
+      <c r="I6" s="17">
+        <v>0</v>
+      </c>
       <c r="J6" s="32">
         <f>G6+I6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+        <v>3.4722222222222099E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15">
+      <c r="A7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="7">
+        <v>30</v>
+      </c>
+      <c r="C7" s="7">
+        <v>41</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.4909722222222222</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="G7" s="8">
         <f>F7-E7</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="8"/>
+        <v>2.9861111111111172E-2</v>
+      </c>
+      <c r="H7" s="7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="J7" s="19">
         <f>G7+I7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <v>5.06944444444445E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15">
       <c r="A8" s="18"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1826,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15">
       <c r="A9" s="20"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1844,9 +1882,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15.75" thickBot="1">
       <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
@@ -1862,138 +1900,138 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15.75" thickBot="1">
       <c r="A11" s="50" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="26">
         <f>SUM(B6:B10)</f>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C11" s="26">
         <f>SUM(C6:C10)</f>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="D11" s="27">
         <f>SUM(D6:D10)</f>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="26"/>
       <c r="G11" s="27">
         <f>SUM(G6:G10)</f>
-        <v>0</v>
+        <v>3.3333333333333381E-2</v>
       </c>
       <c r="H11" s="28">
         <f>SUM(H6:H10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="29">
         <f>SUM(I6:I10)</f>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="J11" s="30">
         <f>SUM(J6:J10)</f>
-        <v>0</v>
+        <v>5.416666666666671E-2</v>
       </c>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1">
       <c r="A12" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="21" t="str">
+      <c r="B12" s="21">
         <f>IF(EXACT($C$11, 0),"-",ABS($B$11-$C$11)/$C$11)</f>
-        <v>-</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="D12" s="5"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="13.5" thickBot="1"/>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1">
       <c r="A14" s="44" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="45"/>
     </row>
-    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15">
       <c r="A15" s="33" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="34">
         <f>C11</f>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="C15" s="9"/>
     </row>
-    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15">
       <c r="A16" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="36" t="str">
+      <c r="B16" s="36">
         <f>IF(EXACT($B$15,0),"-",$B$15/((J11-INT(J11))*24))</f>
-        <v>-</v>
+        <v>36.923076923076891</v>
       </c>
       <c r="C16" s="9"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15.75" thickBot="1">
       <c r="A17" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="36" t="str">
+      <c r="B17" s="36">
         <f>IF(EXACT($B$15,0),"-",H11/($B$15/10))</f>
-        <v>-</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15.75" thickBot="1">
       <c r="A18" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="38" t="str">
+      <c r="B18" s="38">
         <f>IF(EXACT($B$15,0),"-",H11/$B$15)</f>
-        <v>-</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="C18" s="46" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15">
       <c r="A19" s="37" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="39">
         <f>I11</f>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="C19" s="42">
         <f>IF(EXACT(J11,0),5%,B19/J11)</f>
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.3846153846153843</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1">
       <c r="A20" s="40" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="41">
         <f>G11</f>
-        <v>0</v>
+        <v>3.3333333333333381E-2</v>
       </c>
       <c r="C20" s="43">
         <f>IF(EXACT(J11,0),95%,B20/J11)</f>
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.61538461538461575</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="D22" s="6"/>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:4">
       <c r="C35" s="4"/>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:4">
       <c r="D37" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Se actualizaron las metricas. - Se implemento cola dinamica. - Se refactorizo el nombre de algunos miembros privados en pila y cola dinamica.
</commit_message>
<xml_diff>
--- a/practica2/trunk/TDAs/doc/metricas/metricas_cola.xlsx
+++ b/practica2/trunk/TDAs/doc/metricas/metricas_cola.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Implementar Cola Estatica</t>
+  </si>
+  <si>
+    <t>implementar Cola Dinamica</t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1098,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.3846153846153843</c:v>
+                  <c:v>0.26086956521739113</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.61538461538461575</c:v>
+                  <c:v>0.73913043478260887</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1119,7 +1122,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.51180555555555562" footer="0.51180555555555562"/>
+    <c:pageMargins b="1" l="0.75000000000000022" r="0.75000000000000022" t="1" header="0.51180555555555562" footer="0.51180555555555562"/>
     <c:pageSetup firstPageNumber="0"/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1198,7 +1201,7 @@
         <a:effectLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="77"/>
               </a:solidFill>
@@ -1208,7 +1211,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1265,7 +1268,7 @@
         <a:effectLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="77"/>
               </a:solidFill>
@@ -1275,7 +1278,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1612,7 +1615,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1654,7 +1657,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1678,7 +1681,7 @@
   <dimension ref="A1:IU37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.28515625" defaultRowHeight="12.75"/>
@@ -1847,21 +1850,37 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15">
-      <c r="A8" s="18"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="A8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="7">
+        <v>40</v>
+      </c>
+      <c r="C8" s="7">
+        <v>36</v>
+      </c>
+      <c r="D8" s="8">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.11944444444444445</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.1451388888888889</v>
+      </c>
       <c r="G8" s="8">
         <f>F8-E8</f>
+        <v>2.569444444444445E-2</v>
+      </c>
+      <c r="H8" s="7">
         <v>0</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="8"/>
+      <c r="I8" s="8">
+        <v>0</v>
+      </c>
       <c r="J8" s="19">
         <f>G8+I8</f>
-        <v>0</v>
+        <v>2.569444444444445E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15">
@@ -1906,21 +1925,21 @@
       </c>
       <c r="B11" s="26">
         <f>SUM(B6:B10)</f>
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="C11" s="26">
         <f>SUM(C6:C10)</f>
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="D11" s="27">
         <f>SUM(D6:D10)</f>
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="26"/>
       <c r="G11" s="27">
         <f>SUM(G6:G10)</f>
-        <v>3.3333333333333381E-2</v>
+        <v>5.9027777777777832E-2</v>
       </c>
       <c r="H11" s="28">
         <f>SUM(H6:H10)</f>
@@ -1932,7 +1951,7 @@
       </c>
       <c r="J11" s="30">
         <f>SUM(J6:J10)</f>
-        <v>5.416666666666671E-2</v>
+        <v>7.986111111111116E-2</v>
       </c>
       <c r="K11" s="4"/>
     </row>
@@ -1942,7 +1961,7 @@
       </c>
       <c r="B12" s="21">
         <f>IF(EXACT($C$11, 0),"-",ABS($B$11-$C$11)/$C$11)</f>
-        <v>0.22916666666666666</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D12" s="5"/>
       <c r="J12" s="3"/>
@@ -1960,7 +1979,7 @@
       </c>
       <c r="B15" s="34">
         <f>C11</f>
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C15" s="9"/>
     </row>
@@ -1970,7 +1989,7 @@
       </c>
       <c r="B16" s="36">
         <f>IF(EXACT($B$15,0),"-",$B$15/((J11-INT(J11))*24))</f>
-        <v>36.923076923076891</v>
+        <v>43.826086956521713</v>
       </c>
       <c r="C16" s="9"/>
     </row>
@@ -1980,7 +1999,7 @@
       </c>
       <c r="B17" s="36">
         <f>IF(EXACT($B$15,0),"-",H11/($B$15/10))</f>
-        <v>0.20833333333333334</v>
+        <v>0.11904761904761904</v>
       </c>
       <c r="C17" s="9"/>
     </row>
@@ -1990,7 +2009,7 @@
       </c>
       <c r="B18" s="38">
         <f>IF(EXACT($B$15,0),"-",H11/$B$15)</f>
-        <v>2.0833333333333332E-2</v>
+        <v>1.1904761904761904E-2</v>
       </c>
       <c r="C18" s="46" t="s">
         <v>19</v>
@@ -2006,7 +2025,7 @@
       </c>
       <c r="C19" s="42">
         <f>IF(EXACT(J11,0),5%,B19/J11)</f>
-        <v>0.3846153846153843</v>
+        <v>0.26086956521739113</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1">
@@ -2015,11 +2034,11 @@
       </c>
       <c r="B20" s="41">
         <f>G11</f>
-        <v>3.3333333333333381E-2</v>
+        <v>5.9027777777777832E-2</v>
       </c>
       <c r="C20" s="43">
         <f>IF(EXACT(J11,0),95%,B20/J11)</f>
-        <v>0.61538461538461575</v>
+        <v>0.73913043478260887</v>
       </c>
     </row>
     <row r="21" spans="1:4">

</xml_diff>

<commit_message>
Establecida PilaHL como análogo de ColaHL. Actualizadas las métricas y diagramas UML. Actualizadas las conclusiones.
</commit_message>
<xml_diff>
--- a/practica2/trunk/TDAs/doc/metricas/metricas_cola.xlsx
+++ b/practica2/trunk/TDAs/doc/metricas/metricas_cola.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="329"/>
+    <workbookView xWindow="915" yWindow="1785" windowWidth="16380" windowHeight="8190" tabRatio="329"/>
   </bookViews>
   <sheets>
     <sheet name="Metricas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -101,16 +101,22 @@
   </si>
   <si>
     <t>implementar Cola Dinamica</t>
+  </si>
+  <si>
+    <t>Implementar ColaCL</t>
+  </si>
+  <si>
+    <t>Implementar ColaHL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -221,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -522,19 +528,6 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -679,7 +672,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -731,35 +724,32 @@
     <xf numFmtId="164" fontId="5" fillId="5" borderId="21" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="21" fontId="5" fillId="5" borderId="22" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="4" fillId="2" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="21" fontId="4" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="21" fontId="4" fillId="2" borderId="25" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="25" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="21" fontId="5" fillId="5" borderId="27" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="21" fontId="5" fillId="5" borderId="26" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="15" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyBorder="1"/>
@@ -768,31 +758,31 @@
     </xf>
     <xf numFmtId="10" fontId="4" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="29" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="29" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="4" fillId="3" borderId="30" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="31" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="25" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="24" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
@@ -900,8 +890,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:date1904 val="0"/>
+  <c:lang val="es-AR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -920,7 +919,9 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -930,6 +931,7 @@
           <c:order val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
@@ -974,6 +976,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
@@ -1072,14 +1075,20 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-AR"/>
               </a:p>
             </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
             <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Metricas!$A$19:$A$20</c:f>
+              <c:f>Metricas!$A$22:$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1093,22 +1102,28 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Metricas!$C$19:$C$20</c:f>
+              <c:f>Metricas!$C$22:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.26086956521739113</c:v>
+                  <c:v>9.6153846153846118E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.73913043478260887</c:v>
+                  <c:v>0.90384615384615385</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
           <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
         </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
@@ -1116,9 +1131,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
@@ -1135,13 +1152,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1201,7 +1218,7 @@
         <a:effectLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="77"/>
               </a:solidFill>
@@ -1211,7 +1228,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1268,7 +1285,7 @@
         <a:effectLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="77"/>
               </a:solidFill>
@@ -1278,7 +1295,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1615,7 +1632,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1657,7 +1674,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1676,15 +1693,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:IU37"/>
+  <dimension ref="A1:IU40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="34.28515625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="34.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" style="1" customWidth="1"/>
@@ -1699,30 +1716,30 @@
     <col min="11" max="255" width="34.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="53" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="15">
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="55">
+      <c r="B2" s="54">
         <v>3.472222222222222E-3</v>
       </c>
       <c r="C2" s="11">
@@ -1736,60 +1753,66 @@
         <v>0.4826388888888889</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="14"/>
+      <c r="B3" s="14">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="C3" s="14">
         <f>E3-D3</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15"/>
-    </row>
-    <row r="4" spans="1:11" ht="13.5" thickBot="1"/>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A5" s="47" t="s">
+        <v>4.8611111111110938E-3</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0.53125</v>
+      </c>
+      <c r="E3" s="15">
+        <v>0.53611111111111109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="48" t="s">
+      <c r="H5" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="48" t="s">
+      <c r="I5" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="49" t="s">
+      <c r="J5" s="48" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15">
-      <c r="A6" s="31" t="s">
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="16">
         <v>7</v>
       </c>
       <c r="C6" s="16">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="17">
         <v>6.9444444444444441E-3</v>
@@ -1810,20 +1833,20 @@
       <c r="I6" s="17">
         <v>0</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J6" s="31">
         <f>G6+I6</f>
         <v>3.4722222222222099E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15">
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="7">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C7" s="7">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="D7" s="8">
         <v>1.3888888888888888E-2</v>
@@ -1842,22 +1865,22 @@
         <v>1</v>
       </c>
       <c r="I7" s="8">
-        <v>2.0833333333333332E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="J7" s="19">
         <f>G7+I7</f>
-        <v>5.06944444444445E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15">
+        <v>4.0277777777777836E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="7">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C8" s="7">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="D8" s="8">
         <v>2.0833333333333332E-2</v>
@@ -1883,175 +1906,261 @@
         <v>2.569444444444445E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15">
-      <c r="A9" s="20"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="7">
+        <v>40</v>
+      </c>
+      <c r="C9" s="7">
+        <v>39</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.67499999999999993</v>
+      </c>
       <c r="G9" s="8">
-        <f>F9-E9</f>
+        <f t="shared" ref="G9:G13" si="0">F9-E9</f>
+        <v>1.2499999999999956E-2</v>
+      </c>
+      <c r="H9" s="7">
         <v>0</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="8"/>
+      <c r="I9" s="8">
+        <v>0</v>
+      </c>
       <c r="J9" s="19">
-        <f>G9+I9</f>
+        <f t="shared" ref="J9:J13" si="1">G9+I9</f>
+        <v>1.2499999999999956E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="7">
+        <v>80</v>
+      </c>
+      <c r="C10" s="7">
+        <v>98</v>
+      </c>
+      <c r="D10" s="8">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.52847222222222223</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="0"/>
+        <v>2.6388888888888906E-2</v>
+      </c>
+      <c r="H10" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A10" s="22"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24">
-        <f>F10-E10</f>
+      <c r="I10" s="8">
         <v>0</v>
       </c>
-      <c r="H10" s="23"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="25">
-        <f>G10+I10</f>
+      <c r="J10" s="19">
+        <f t="shared" si="1"/>
+        <v>2.6388888888888906E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A11" s="50" t="s">
+      <c r="H11" s="7"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="26">
-        <f>SUM(B6:B10)</f>
-        <v>77</v>
-      </c>
-      <c r="C11" s="26">
-        <f>SUM(C6:C10)</f>
-        <v>84</v>
-      </c>
-      <c r="D11" s="27">
-        <f>SUM(D6:D10)</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="27">
-        <f>SUM(G6:G10)</f>
-        <v>5.9027777777777832E-2</v>
-      </c>
-      <c r="H11" s="28">
-        <f>SUM(H6:H10)</f>
+      <c r="B14" s="25">
+        <f>SUM(B6:B13)</f>
+        <v>257</v>
+      </c>
+      <c r="C14" s="25">
+        <f>SUM(C6:C13)</f>
+        <v>287</v>
+      </c>
+      <c r="D14" s="26">
+        <f>SUM(D6:D13)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="26">
+        <f>SUM(G6:G13)</f>
+        <v>9.7916666666666693E-2</v>
+      </c>
+      <c r="H14" s="27">
+        <f>SUM(H6:H13)</f>
         <v>1</v>
       </c>
-      <c r="I11" s="29">
-        <f>SUM(I6:I10)</f>
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="J11" s="30">
-        <f>SUM(J6:J10)</f>
-        <v>7.986111111111116E-2</v>
-      </c>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A12" s="51" t="s">
+      <c r="I14" s="28">
+        <f>SUM(I6:I13)</f>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="J14" s="29">
+        <f>SUM(J6:J13)</f>
+        <v>0.10833333333333336</v>
+      </c>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="21">
-        <f>IF(EXACT($C$11, 0),"-",ABS($B$11-$C$11)/$C$11)</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" ht="13.5" thickBot="1"/>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A14" s="44" t="s">
+      <c r="B15" s="21">
+        <f>IF(EXACT($C$14, 0),"-",ABS($B$14-$C$14)/$C$14)</f>
+        <v>0.10452961672473868</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="45"/>
-    </row>
-    <row r="15" spans="1:11" ht="15">
-      <c r="A15" s="33" t="s">
+      <c r="B17" s="44"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="34">
-        <f>C11</f>
-        <v>84</v>
-      </c>
-      <c r="C15" s="9"/>
-    </row>
-    <row r="16" spans="1:11" ht="15">
-      <c r="A16" s="35" t="s">
+      <c r="B18" s="33">
+        <f>C14</f>
+        <v>287</v>
+      </c>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="36">
-        <f>IF(EXACT($B$15,0),"-",$B$15/((J11-INT(J11))*24))</f>
-        <v>43.826086956521713</v>
-      </c>
-      <c r="C16" s="9"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A17" s="37" t="s">
+      <c r="B19" s="35">
+        <f>IF(EXACT($B$18,0),"-",$B$18/((J14-INT(J14))*24))</f>
+        <v>110.38461538461536</v>
+      </c>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="36">
-        <f>IF(EXACT($B$15,0),"-",H11/($B$15/10))</f>
-        <v>0.11904761904761904</v>
-      </c>
-      <c r="C17" s="9"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A18" s="37" t="s">
+      <c r="B20" s="35">
+        <f>IF(EXACT($B$18,0),"-",H14/($B$18/10))</f>
+        <v>3.484320557491289E-2</v>
+      </c>
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="38">
-        <f>IF(EXACT($B$15,0),"-",H11/$B$15)</f>
-        <v>1.1904761904761904E-2</v>
-      </c>
-      <c r="C18" s="46" t="s">
+      <c r="B21" s="37">
+        <f>IF(EXACT($B$18,0),"-",H14/$B$18)</f>
+        <v>3.4843205574912892E-3</v>
+      </c>
+      <c r="C21" s="45" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15">
-      <c r="A19" s="37" t="s">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="39">
-        <f>I11</f>
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C19" s="42">
-        <f>IF(EXACT(J11,0),5%,B19/J11)</f>
-        <v>0.26086956521739113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A20" s="40" t="s">
+      <c r="B22" s="38">
+        <f>I14</f>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C22" s="41">
+        <f>IF(EXACT(J14,0),5%,B22/J14)</f>
+        <v>9.6153846153846118E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="41">
-        <f>G11</f>
-        <v>5.9027777777777832E-2</v>
-      </c>
-      <c r="C20" s="43">
-        <f>IF(EXACT(J11,0),95%,B20/J11)</f>
-        <v>0.73913043478260887</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="D22" s="6"/>
-    </row>
-    <row r="35" spans="3:4">
-      <c r="C35" s="4"/>
-    </row>
-    <row r="37" spans="3:4">
-      <c r="D37" s="4"/>
+      <c r="B23" s="40">
+        <f>G14</f>
+        <v>9.7916666666666693E-2</v>
+      </c>
+      <c r="C23" s="42">
+        <f>IF(EXACT(J14,0),95%,B23/J14)</f>
+        <v>0.90384615384615385</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D25" s="6"/>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C38" s="4"/>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D40" s="4"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Agregado Monticulo, MonticuloMaximo y ColaPrioridad. Actualizadas las métricas. Actualizado el diagrama UML. Agregados contenedores para tests.
</commit_message>
<xml_diff>
--- a/practica2/trunk/TDAs/doc/metricas/metricas_cola.xlsx
+++ b/practica2/trunk/TDAs/doc/metricas/metricas_cola.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="1785" windowWidth="16380" windowHeight="8190" tabRatio="329"/>
+    <workbookView xWindow="15" yWindow="30" windowWidth="28680" windowHeight="12330" tabRatio="329"/>
   </bookViews>
   <sheets>
     <sheet name="Metricas" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -107,6 +107,15 @@
   </si>
   <si>
     <t>Implementar ColaHL</t>
+  </si>
+  <si>
+    <t>Implementar Monticulo</t>
+  </si>
+  <si>
+    <t>Implementar MonticuloMaximo</t>
+  </si>
+  <si>
+    <t>Implementar ColaPrioridad</t>
   </si>
 </sst>
 </file>
@@ -672,7 +681,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -709,9 +718,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="21" fontId="5" fillId="5" borderId="17" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="4" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1088,7 +1094,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Metricas!$A$22:$A$23</c:f>
+              <c:f>Metricas!$A$25:$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1102,15 +1108,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Metricas!$C$22:$C$23</c:f>
+              <c:f>Metricas!$C$25:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.6153846153846118E-2</c:v>
+                  <c:v>7.6923076923076913E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.90384615384615385</c:v>
+                  <c:v>0.92307692307692302</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1152,13 +1158,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1695,10 +1701,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:IU40"/>
+  <dimension ref="A1:IU43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1716,30 +1722,30 @@
     <col min="11" max="255" width="34.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="52" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="54">
+      <c r="B2" s="53">
         <v>3.472222222222222E-3</v>
       </c>
       <c r="C2" s="11">
@@ -1753,7 +1759,7 @@
         <v>0.4826388888888889</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -1771,41 +1777,41 @@
         <v>0.53611111111111109</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46" t="s">
+    <row r="4" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="47" t="s">
+      <c r="G5" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="48" t="s">
+      <c r="J5" s="47" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="16">
@@ -1833,12 +1839,12 @@
       <c r="I6" s="17">
         <v>0</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="30">
         <f>G6+I6</f>
         <v>3.4722222222222099E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>27</v>
       </c>
@@ -1857,8 +1863,8 @@
       <c r="F7" s="8">
         <v>0.52083333333333337</v>
       </c>
-      <c r="G7" s="8">
-        <f>F7-E7</f>
+      <c r="G7" s="17">
+        <f t="shared" ref="G7:G16" si="0">F7-E7</f>
         <v>2.9861111111111172E-2</v>
       </c>
       <c r="H7" s="7">
@@ -1867,12 +1873,12 @@
       <c r="I7" s="8">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="J7" s="19">
-        <f>G7+I7</f>
+      <c r="J7" s="30">
+        <f t="shared" ref="J7:J16" si="1">G7+I7</f>
         <v>4.0277777777777836E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>28</v>
       </c>
@@ -1891,8 +1897,8 @@
       <c r="F8" s="8">
         <v>0.1451388888888889</v>
       </c>
-      <c r="G8" s="8">
-        <f>F8-E8</f>
+      <c r="G8" s="17">
+        <f t="shared" si="0"/>
         <v>2.569444444444445E-2</v>
       </c>
       <c r="H8" s="7">
@@ -1901,12 +1907,12 @@
       <c r="I8" s="8">
         <v>0</v>
       </c>
-      <c r="J8" s="19">
-        <f>G8+I8</f>
+      <c r="J8" s="30">
+        <f t="shared" si="1"/>
         <v>2.569444444444445E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>29</v>
       </c>
@@ -1925,8 +1931,8 @@
       <c r="F9" s="8">
         <v>0.67499999999999993</v>
       </c>
-      <c r="G9" s="8">
-        <f t="shared" ref="G9:G13" si="0">F9-E9</f>
+      <c r="G9" s="17">
+        <f t="shared" si="0"/>
         <v>1.2499999999999956E-2</v>
       </c>
       <c r="H9" s="7">
@@ -1935,12 +1941,12 @@
       <c r="I9" s="8">
         <v>0</v>
       </c>
-      <c r="J9" s="19">
-        <f t="shared" ref="J9:J13" si="1">G9+I9</f>
+      <c r="J9" s="30">
+        <f t="shared" si="1"/>
         <v>1.2499999999999956E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>30</v>
       </c>
@@ -1959,7 +1965,7 @@
       <c r="F10" s="8">
         <v>0.52847222222222223</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="17">
         <f t="shared" si="0"/>
         <v>2.6388888888888906E-2</v>
       </c>
@@ -1969,198 +1975,300 @@
       <c r="I10" s="8">
         <v>0</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="30">
         <f t="shared" si="1"/>
         <v>2.6388888888888906E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8">
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="7">
+        <v>20</v>
+      </c>
+      <c r="C11" s="7">
+        <v>6</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.81180555555555556</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.81597222222222221</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666519E-3</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0</v>
+      </c>
+      <c r="J11" s="30">
+        <f t="shared" si="1"/>
+        <v>4.1666666666666519E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="7">
+        <v>50</v>
+      </c>
+      <c r="C12" s="7">
+        <v>103</v>
+      </c>
+      <c r="D12" s="8">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.81597222222222221</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.87569444444444444</v>
+      </c>
+      <c r="G12" s="17">
+        <f t="shared" si="0"/>
+        <v>5.9722222222222232E-2</v>
+      </c>
+      <c r="H12" s="7">
+        <v>1</v>
+      </c>
+      <c r="I12" s="8">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="J12" s="30">
+        <f t="shared" si="1"/>
+        <v>6.3194444444444456E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="7">
+        <v>40</v>
+      </c>
+      <c r="C13" s="7">
+        <v>47</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.73402777777777783</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.73888888888888893</v>
+      </c>
+      <c r="G13" s="17">
+        <f t="shared" si="0"/>
+        <v>4.8611111111110938E-3</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0</v>
+      </c>
+      <c r="J13" s="30">
+        <f t="shared" si="1"/>
+        <v>4.8611111111110938E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="19">
+      <c r="H14" s="7"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8">
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="19">
+      <c r="H15" s="7"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="8">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="21"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="19">
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49" t="s">
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="25">
-        <f>SUM(B6:B13)</f>
-        <v>257</v>
-      </c>
-      <c r="C14" s="25">
-        <f>SUM(C6:C13)</f>
-        <v>287</v>
-      </c>
-      <c r="D14" s="26">
-        <f>SUM(D6:D13)</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26">
-        <f>SUM(G6:G13)</f>
-        <v>9.7916666666666693E-2</v>
-      </c>
-      <c r="H14" s="27">
-        <f>SUM(H6:H13)</f>
-        <v>1</v>
-      </c>
-      <c r="I14" s="28">
-        <f>SUM(I6:I13)</f>
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="J14" s="29">
-        <f>SUM(J6:J13)</f>
-        <v>0.10833333333333336</v>
-      </c>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="50" t="s">
+      <c r="B17" s="24">
+        <f>SUM(B6:B16)</f>
+        <v>367</v>
+      </c>
+      <c r="C17" s="24">
+        <f>SUM(C6:C16)</f>
+        <v>443</v>
+      </c>
+      <c r="D17" s="25">
+        <f>SUM(D6:D16)</f>
+        <v>0.13888888888888887</v>
+      </c>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="25">
+        <f>SUM(G6:G16)</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="H17" s="26">
+        <f>SUM(H6:H16)</f>
+        <v>2</v>
+      </c>
+      <c r="I17" s="27">
+        <f>SUM(I6:I16)</f>
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="J17" s="28">
+        <f>SUM(J6:J16)</f>
+        <v>0.18055555555555558</v>
+      </c>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="21">
-        <f>IF(EXACT($C$14, 0),"-",ABS($B$14-$C$14)/$C$14)</f>
-        <v>0.10452961672473868</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="43" t="s">
+      <c r="B18" s="20">
+        <f>IF(EXACT($C$17, 0),"-",ABS($B$17-$C$17)/$C$17)</f>
+        <v>0.17155756207674944</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="44"/>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="B20" s="43"/>
+    </row>
+    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="33">
-        <f>C14</f>
-        <v>287</v>
-      </c>
-      <c r="C18" s="9"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="B21" s="32">
+        <f>C17</f>
+        <v>443</v>
+      </c>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="35">
-        <f>IF(EXACT($B$18,0),"-",$B$18/((J14-INT(J14))*24))</f>
-        <v>110.38461538461536</v>
-      </c>
-      <c r="C19" s="9"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="36" t="s">
+      <c r="B22" s="34">
+        <f>IF(EXACT($B$21,0),"-",$B$21/((J17-INT(J17))*24))</f>
+        <v>102.23076923076921</v>
+      </c>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="35">
-        <f>IF(EXACT($B$18,0),"-",H14/($B$18/10))</f>
-        <v>3.484320557491289E-2</v>
-      </c>
-      <c r="C20" s="9"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="36" t="s">
+      <c r="B23" s="34">
+        <f>IF(EXACT($B$21,0),"-",H17/($B$21/10))</f>
+        <v>4.5146726862302484E-2</v>
+      </c>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="37">
-        <f>IF(EXACT($B$18,0),"-",H14/$B$18)</f>
-        <v>3.4843205574912892E-3</v>
-      </c>
-      <c r="C21" s="45" t="s">
+      <c r="B24" s="36">
+        <f>IF(EXACT($B$21,0),"-",H17/$B$21)</f>
+        <v>4.5146726862302479E-3</v>
+      </c>
+      <c r="C24" s="44" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
+    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="38">
-        <f>I14</f>
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="C22" s="41">
-        <f>IF(EXACT(J14,0),5%,B22/J14)</f>
-        <v>9.6153846153846118E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="39" t="s">
+      <c r="B25" s="37">
+        <f>I17</f>
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C25" s="40">
+        <f>IF(EXACT(J17,0),5%,B25/J17)</f>
+        <v>7.6923076923076913E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="40">
-        <f>G14</f>
-        <v>9.7916666666666693E-2</v>
-      </c>
-      <c r="C23" s="42">
-        <f>IF(EXACT(J14,0),95%,B23/J14)</f>
-        <v>0.90384615384615385</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D25" s="6"/>
-    </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C38" s="4"/>
-    </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D40" s="4"/>
+      <c r="B26" s="39">
+        <f>G17</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="C26" s="41">
+        <f>IF(EXACT(J17,0),95%,B26/J17)</f>
+        <v>0.92307692307692302</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D28" s="6"/>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C41" s="4"/>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D43" s="4"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>